<commit_message>
Load data from excel file and SQL server
</commit_message>
<xml_diff>
--- a/LaptopManagement/LaptopManagement/data/LaptopList.xlsx
+++ b/LaptopManagement/LaptopManagement/data/LaptopList.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\dotNET Programming\LaptopManagement\LaptopManagement\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\dotNET Programming\LaptopManagement\LaptopManagement\bin\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AB0B436-51CF-4A0E-85A8-1F2C27DEEF4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FE9435C5-FE0A-4874-8B02-7E12D41C2FF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21195" yWindow="2355" windowWidth="28800" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3795" yWindow="1095" windowWidth="28800" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="37">
   <si>
     <t>LaptopID</t>
   </si>
@@ -60,9 +60,6 @@
     <t>Gaming</t>
   </si>
   <si>
-    <t>2023-03-15</t>
-  </si>
-  <si>
     <t>Intel i5</t>
   </si>
   <si>
@@ -78,9 +75,6 @@
     <t>Business</t>
   </si>
   <si>
-    <t>2022-11-20</t>
-  </si>
-  <si>
     <t>Intel i7</t>
   </si>
   <si>
@@ -93,9 +87,6 @@
     <t>Lenovo ThinkPad</t>
   </si>
   <si>
-    <t>2023-01-05</t>
-  </si>
-  <si>
     <t>AMD Ryzen 5</t>
   </si>
   <si>
@@ -108,9 +99,6 @@
     <t>Ultrabook</t>
   </si>
   <si>
-    <t>2022-09-18</t>
-  </si>
-  <si>
     <t>Intel i3</t>
   </si>
   <si>
@@ -118,9 +106,6 @@
   </si>
   <si>
     <t>Apple MacBook Air</t>
-  </si>
-  <si>
-    <t>2023-07-10</t>
   </si>
   <si>
     <t>Apple M1</t>
@@ -157,6 +142,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="165" formatCode="dd\/mm\/yyyy"/>
+    <numFmt numFmtId="166" formatCode="m/d/yy;@"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -209,11 +198,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -494,10 +488,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -505,7 +499,7 @@
     <col min="1" max="1" width="10.5703125" customWidth="1"/>
     <col min="2" max="2" width="20.7109375" customWidth="1"/>
     <col min="3" max="3" width="16.5703125" customWidth="1"/>
-    <col min="4" max="4" width="22.5703125" customWidth="1"/>
+    <col min="4" max="4" width="22.5703125" style="3" customWidth="1"/>
     <col min="5" max="5" width="14.7109375" customWidth="1"/>
     <col min="6" max="6" width="12" customWidth="1"/>
     <col min="7" max="7" width="12.5703125" customWidth="1"/>
@@ -523,7 +517,7 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
@@ -544,7 +538,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B2" t="s">
         <v>9</v>
@@ -552,140 +546,155 @@
       <c r="C2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="3">
+        <v>45000</v>
+      </c>
+      <c r="E2" t="s">
         <v>11</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G2" t="s">
         <v>12</v>
-      </c>
-      <c r="F2" t="s">
-        <v>34</v>
-      </c>
-      <c r="G2" t="s">
-        <v>13</v>
       </c>
       <c r="H2">
         <v>800</v>
       </c>
       <c r="I2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
         <v>15</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" s="3">
+        <v>44155</v>
+      </c>
+      <c r="E3" t="s">
         <v>16</v>
       </c>
-      <c r="D3" t="s">
+      <c r="F3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G3" t="s">
         <v>17</v>
-      </c>
-      <c r="E3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" t="s">
-        <v>35</v>
-      </c>
-      <c r="G3" t="s">
-        <v>19</v>
       </c>
       <c r="H3">
         <v>1200</v>
       </c>
       <c r="I3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" t="s">
-        <v>22</v>
+        <v>15</v>
+      </c>
+      <c r="D4" s="3">
+        <v>44931</v>
       </c>
       <c r="E4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F4" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="G4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H4">
         <v>950</v>
       </c>
       <c r="I4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D5" t="s">
-        <v>27</v>
+        <v>23</v>
+      </c>
+      <c r="D5" s="3">
+        <v>44822</v>
       </c>
       <c r="E5" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="G5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H5">
         <v>700</v>
       </c>
       <c r="I5" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D6" t="s">
-        <v>31</v>
+        <v>23</v>
+      </c>
+      <c r="D6" s="3">
+        <v>45117</v>
       </c>
       <c r="E6" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="F6" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="G6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H6">
         <v>1300</v>
       </c>
       <c r="I6" t="s">
-        <v>33</v>
-      </c>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D10" s="4"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D11" s="4"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D12" s="4"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D13" s="4"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D14" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>